<commit_message>
Update Entry date column in CYRS Review sheet & delete non-related point Signed-off-by: Abdelrahman-Omar-Ali <a.abdelwahed20@gmail.com>
</commit_message>
<xml_diff>
--- a/Input documents/CYRS_Review.xlsx
+++ b/Input documents/CYRS_Review.xlsx
@@ -12,7 +12,7 @@
     <sheet name="Cross review points " sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="false" localSheetId="1" name="_Toc30697436" vbProcedure="false">'Cross review points '!$F$8</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_Toc30697436" vbProcedure="false">#REF!</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="51">
   <si>
     <t xml:space="preserve">Project Name </t>
   </si>
@@ -104,7 +104,7 @@
     <t xml:space="preserve">Comment</t>
   </si>
   <si>
-    <t xml:space="preserve">29/01/2019</t>
+    <t xml:space="preserve">29/01/2020</t>
   </si>
   <si>
     <t xml:space="preserve">A.Ali</t>
@@ -128,27 +128,18 @@
     <t xml:space="preserve">Open</t>
   </si>
   <si>
-    <t xml:space="preserve">29/01/2020</t>
-  </si>
-  <si>
     <t xml:space="preserve">All pages</t>
   </si>
   <si>
     <t xml:space="preserve">Redundancy in Version field besides Date in header table. </t>
   </si>
   <si>
-    <t xml:space="preserve">29/01/2021</t>
-  </si>
-  <si>
     <t xml:space="preserve">Contents</t>
   </si>
   <si>
     <t xml:space="preserve">Update Table of Content numbering specially for Functional Requirements section. </t>
   </si>
   <si>
-    <t xml:space="preserve">29/01/2022</t>
-  </si>
-  <si>
     <t xml:space="preserve">ALL</t>
   </si>
   <si>
@@ -156,9 +147,6 @@
   </si>
   <si>
     <t xml:space="preserve">Refused</t>
-  </si>
-  <si>
-    <t xml:space="preserve">29/01/2023</t>
   </si>
   <si>
     <t xml:space="preserve">Functional Requirements</t>
@@ -187,6 +175,7 @@
         <sz val="11"/>
         <rFont val="Calibri Light"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> </t>
     </r>
@@ -196,20 +185,10 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">You can list all HW Req in hardware software interface document (HSI) , because in this requirement nothing related to HW as it more likely SW, so you need to update its #Imp to be only SW and if you see that you need a HW requirement defined this part of system, you could add it in HSI. </t>
     </r>
-  </si>
-  <si>
-    <t xml:space="preserve">29/01/2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Req_ PO3_DGW_CYRS_02_V01 : 
-Here you want to defient he HW req then the goal from HW is to describ the HW , but in the req nothing related to HW as it more likely SW 
-So if you want to describ the HW then for Ex : you can say The system shall use 16*2 display to show different mode ,, and so on </t>
-  </si>
-  <si>
-    <t xml:space="preserve">29/01/2025</t>
   </si>
   <si>
     <t xml:space="preserve">REQ_PO2EBL_CYRS_04_V02: 
@@ -299,6 +278,7 @@
       <sz val="11"/>
       <name val="Calibri Light"/>
       <family val="1"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -483,7 +463,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="34">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -576,16 +556,12 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="10" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="10" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="10" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -772,7 +748,7 @@
       <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.55078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="32.29"/>
   </cols>
@@ -1011,20 +987,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L48"/>
+  <dimension ref="A1:L1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I9" activeCellId="0" sqref="I9"/>
+      <selection pane="topLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.55078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="11.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="24"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="100.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="100.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="8" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="174.28"/>
   </cols>
@@ -1087,7 +1063,7 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="17" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="B3" s="18" t="s">
         <v>27</v>
@@ -1099,10 +1075,10 @@
         <v>29</v>
       </c>
       <c r="E3" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="F3" s="21" t="s">
         <v>35</v>
-      </c>
-      <c r="F3" s="21" t="s">
-        <v>36</v>
       </c>
       <c r="G3" s="22" t="s">
         <v>32</v>
@@ -1114,7 +1090,7 @@
     </row>
     <row r="4" customFormat="false" ht="20.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="17" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="B4" s="18" t="s">
         <v>27</v>
@@ -1126,10 +1102,10 @@
         <v>29</v>
       </c>
       <c r="E4" s="20" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F4" s="21" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G4" s="22" t="s">
         <v>32</v>
@@ -1142,24 +1118,24 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="17" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="B5" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="C5" s="23" t="s">
+      <c r="C5" s="19" t="s">
         <v>28</v>
       </c>
       <c r="D5" s="18" t="s">
         <v>29</v>
       </c>
       <c r="E5" s="20" t="s">
-        <v>41</v>
-      </c>
-      <c r="F5" s="24" t="s">
-        <v>42</v>
+        <v>38</v>
+      </c>
+      <c r="F5" s="23" t="s">
+        <v>39</v>
       </c>
       <c r="G5" s="22" t="s">
         <v>32</v>
@@ -1169,27 +1145,27 @@
       </c>
       <c r="I5" s="22"/>
       <c r="K5" s="0" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="64.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="17" t="s">
-        <v>44</v>
+      <c r="A6" s="24" t="s">
+        <v>26</v>
       </c>
       <c r="B6" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="C6" s="23" t="s">
+      <c r="C6" s="19" t="s">
         <v>28</v>
       </c>
       <c r="D6" s="18" t="s">
         <v>29</v>
       </c>
       <c r="E6" s="20" t="s">
-        <v>45</v>
-      </c>
-      <c r="F6" s="24" t="s">
-        <v>46</v>
+        <v>41</v>
+      </c>
+      <c r="F6" s="23" t="s">
+        <v>42</v>
       </c>
       <c r="G6" s="22" t="s">
         <v>32</v>
@@ -1200,23 +1176,23 @@
       <c r="I6" s="22"/>
     </row>
     <row r="7" customFormat="false" ht="52.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="17" t="s">
-        <v>44</v>
+      <c r="A7" s="24" t="s">
+        <v>26</v>
       </c>
       <c r="B7" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="23" t="s">
+      <c r="C7" s="19" t="s">
         <v>28</v>
       </c>
       <c r="D7" s="18" t="s">
         <v>29</v>
       </c>
       <c r="E7" s="20" t="s">
-        <v>47</v>
-      </c>
-      <c r="F7" s="24" t="s">
-        <v>48</v>
+        <v>43</v>
+      </c>
+      <c r="F7" s="23" t="s">
+        <v>44</v>
       </c>
       <c r="G7" s="22" t="s">
         <v>32</v>
@@ -1224,26 +1200,26 @@
       <c r="H7" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="I7" s="25"/>
-    </row>
-    <row r="8" customFormat="false" ht="60" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="17" t="s">
-        <v>49</v>
+      <c r="I7" s="20"/>
+    </row>
+    <row r="8" customFormat="false" ht="57.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="24" t="s">
+        <v>26</v>
       </c>
       <c r="B8" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="C8" s="23" t="s">
+      <c r="C8" s="19" t="s">
         <v>28</v>
       </c>
       <c r="D8" s="18" t="s">
         <v>29</v>
       </c>
       <c r="E8" s="20" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="F8" s="21" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="G8" s="22" t="s">
         <v>32</v>
@@ -1251,51 +1227,32 @@
       <c r="H8" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="I8" s="25"/>
+      <c r="I8" s="20"/>
       <c r="K8" s="0" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="57.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="17" t="s">
-        <v>51</v>
-      </c>
-      <c r="B9" s="18" t="s">
-        <v>27</v>
-      </c>
-      <c r="C9" s="23" t="s">
-        <v>28</v>
-      </c>
-      <c r="D9" s="18" t="s">
-        <v>29</v>
-      </c>
-      <c r="E9" s="20" t="s">
-        <v>41</v>
-      </c>
-      <c r="F9" s="21" t="s">
-        <v>52</v>
-      </c>
-      <c r="G9" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="H9" s="22" t="s">
-        <v>33</v>
-      </c>
-      <c r="I9" s="25"/>
-      <c r="K9" s="0" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="17"/>
+        <v>46</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="17"/>
+      <c r="B9" s="18"/>
+      <c r="C9" s="19"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="20"/>
+      <c r="F9" s="21"/>
+      <c r="G9" s="22"/>
+      <c r="H9" s="22"/>
+      <c r="I9" s="20"/>
+    </row>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="18"/>
       <c r="B10" s="18"/>
-      <c r="C10" s="23"/>
+      <c r="C10" s="19"/>
       <c r="D10" s="18"/>
       <c r="E10" s="20"/>
       <c r="F10" s="21"/>
       <c r="G10" s="22"/>
       <c r="H10" s="22"/>
-      <c r="I10" s="25"/>
+      <c r="I10" s="20"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="18"/>
@@ -1306,7 +1263,13 @@
       <c r="F11" s="21"/>
       <c r="G11" s="22"/>
       <c r="H11" s="22"/>
-      <c r="I11" s="25"/>
+      <c r="I11" s="20"/>
+      <c r="K11" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="L11" s="0" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="18"/>
@@ -1317,12 +1280,12 @@
       <c r="F12" s="21"/>
       <c r="G12" s="22"/>
       <c r="H12" s="22"/>
-      <c r="I12" s="25"/>
+      <c r="I12" s="20"/>
       <c r="K12" s="0" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="L12" s="0" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1334,13 +1297,7 @@
       <c r="F13" s="21"/>
       <c r="G13" s="22"/>
       <c r="H13" s="22"/>
-      <c r="I13" s="25"/>
-      <c r="K13" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="L13" s="0" t="s">
-        <v>57</v>
-      </c>
+      <c r="I13" s="20"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="18"/>
@@ -1351,7 +1308,7 @@
       <c r="F14" s="21"/>
       <c r="G14" s="22"/>
       <c r="H14" s="22"/>
-      <c r="I14" s="25"/>
+      <c r="I14" s="20"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="18"/>
@@ -1362,371 +1319,361 @@
       <c r="F15" s="21"/>
       <c r="G15" s="22"/>
       <c r="H15" s="22"/>
-      <c r="I15" s="25"/>
+      <c r="I15" s="20"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="18"/>
-      <c r="B16" s="18"/>
-      <c r="C16" s="19"/>
-      <c r="D16" s="18"/>
-      <c r="E16" s="20"/>
-      <c r="F16" s="21"/>
+      <c r="A16" s="25"/>
+      <c r="B16" s="26"/>
+      <c r="C16" s="26"/>
+      <c r="D16" s="27"/>
+      <c r="E16" s="28"/>
+      <c r="F16" s="29"/>
       <c r="G16" s="22"/>
       <c r="H16" s="22"/>
-      <c r="I16" s="25"/>
+      <c r="I16" s="30"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="26"/>
-      <c r="B17" s="27"/>
-      <c r="C17" s="27"/>
-      <c r="D17" s="28"/>
-      <c r="E17" s="29"/>
-      <c r="F17" s="30"/>
+      <c r="A17" s="25"/>
+      <c r="B17" s="26"/>
+      <c r="C17" s="26"/>
+      <c r="D17" s="27"/>
+      <c r="E17" s="28"/>
+      <c r="F17" s="29"/>
       <c r="G17" s="22"/>
       <c r="H17" s="22"/>
-      <c r="I17" s="31"/>
+      <c r="I17" s="30"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="26"/>
-      <c r="B18" s="27"/>
+      <c r="A18" s="25"/>
+      <c r="B18" s="26"/>
       <c r="C18" s="27"/>
-      <c r="D18" s="28"/>
-      <c r="E18" s="29"/>
-      <c r="F18" s="30"/>
+      <c r="D18" s="18"/>
+      <c r="E18" s="31"/>
+      <c r="F18" s="29"/>
       <c r="G18" s="22"/>
       <c r="H18" s="22"/>
-      <c r="I18" s="31"/>
+      <c r="I18" s="30"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="26"/>
-      <c r="B19" s="27"/>
-      <c r="C19" s="28"/>
+      <c r="A19" s="25"/>
+      <c r="B19" s="26"/>
+      <c r="C19" s="27"/>
       <c r="D19" s="18"/>
-      <c r="E19" s="32"/>
-      <c r="F19" s="30"/>
+      <c r="E19" s="31"/>
+      <c r="F19" s="32"/>
       <c r="G19" s="22"/>
       <c r="H19" s="22"/>
-      <c r="I19" s="31"/>
+      <c r="I19" s="30"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="26"/>
-      <c r="B20" s="27"/>
-      <c r="C20" s="28"/>
+      <c r="A20" s="25"/>
+      <c r="B20" s="26"/>
+      <c r="C20" s="27"/>
       <c r="D20" s="18"/>
-      <c r="E20" s="32"/>
-      <c r="F20" s="33"/>
+      <c r="E20" s="31"/>
+      <c r="F20" s="32"/>
       <c r="G20" s="22"/>
       <c r="H20" s="22"/>
-      <c r="I20" s="31"/>
+      <c r="I20" s="30"/>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="26"/>
-      <c r="B21" s="27"/>
-      <c r="C21" s="28"/>
+      <c r="A21" s="25"/>
+      <c r="B21" s="26"/>
+      <c r="C21" s="27"/>
       <c r="D21" s="18"/>
-      <c r="E21" s="32"/>
-      <c r="F21" s="33"/>
+      <c r="E21" s="31"/>
+      <c r="F21" s="32"/>
       <c r="G21" s="22"/>
       <c r="H21" s="22"/>
-      <c r="I21" s="31"/>
+      <c r="I21" s="30"/>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="26"/>
-      <c r="B22" s="27"/>
-      <c r="C22" s="28"/>
+      <c r="A22" s="25"/>
+      <c r="B22" s="26"/>
+      <c r="C22" s="27"/>
       <c r="D22" s="18"/>
-      <c r="E22" s="32"/>
-      <c r="F22" s="33"/>
+      <c r="E22" s="31"/>
+      <c r="F22" s="32"/>
       <c r="G22" s="22"/>
       <c r="H22" s="22"/>
-      <c r="I22" s="31"/>
+      <c r="I22" s="30"/>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="26"/>
-      <c r="B23" s="27"/>
-      <c r="C23" s="28"/>
+      <c r="A23" s="25"/>
+      <c r="B23" s="26"/>
+      <c r="C23" s="27"/>
       <c r="D23" s="18"/>
-      <c r="E23" s="32"/>
-      <c r="F23" s="33"/>
+      <c r="E23" s="31"/>
+      <c r="F23" s="32"/>
       <c r="G23" s="22"/>
       <c r="H23" s="22"/>
-      <c r="I23" s="31"/>
+      <c r="I23" s="30"/>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="26"/>
-      <c r="B24" s="27"/>
-      <c r="C24" s="28"/>
+      <c r="A24" s="25"/>
+      <c r="B24" s="26"/>
+      <c r="C24" s="27"/>
       <c r="D24" s="18"/>
-      <c r="E24" s="32"/>
-      <c r="F24" s="33"/>
+      <c r="E24" s="31"/>
+      <c r="F24" s="32"/>
       <c r="G24" s="22"/>
       <c r="H24" s="22"/>
-      <c r="I24" s="31"/>
+      <c r="I24" s="30"/>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="26"/>
-      <c r="B25" s="27"/>
-      <c r="C25" s="28"/>
+      <c r="A25" s="25"/>
+      <c r="B25" s="26"/>
+      <c r="C25" s="27"/>
       <c r="D25" s="18"/>
-      <c r="E25" s="32"/>
-      <c r="F25" s="33"/>
+      <c r="E25" s="31"/>
+      <c r="F25" s="32"/>
       <c r="G25" s="22"/>
       <c r="H25" s="22"/>
-      <c r="I25" s="31"/>
+      <c r="I25" s="30"/>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="26"/>
-      <c r="B26" s="27"/>
-      <c r="C26" s="28"/>
+      <c r="A26" s="25"/>
+      <c r="B26" s="26"/>
+      <c r="C26" s="27"/>
       <c r="D26" s="18"/>
-      <c r="E26" s="32"/>
-      <c r="F26" s="33"/>
+      <c r="E26" s="31"/>
+      <c r="F26" s="32"/>
       <c r="G26" s="22"/>
       <c r="H26" s="22"/>
-      <c r="I26" s="31"/>
+      <c r="I26" s="30"/>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="26"/>
-      <c r="B27" s="27"/>
-      <c r="C27" s="28"/>
+      <c r="A27" s="25"/>
+      <c r="B27" s="26"/>
+      <c r="C27" s="27"/>
       <c r="D27" s="18"/>
-      <c r="E27" s="32"/>
-      <c r="F27" s="33"/>
+      <c r="E27" s="31"/>
+      <c r="F27" s="32"/>
       <c r="G27" s="22"/>
       <c r="H27" s="22"/>
-      <c r="I27" s="31"/>
+      <c r="I27" s="30"/>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="26"/>
+      <c r="A28" s="27"/>
       <c r="B28" s="27"/>
-      <c r="C28" s="28"/>
-      <c r="D28" s="18"/>
-      <c r="E28" s="32"/>
-      <c r="F28" s="33"/>
+      <c r="C28" s="27"/>
+      <c r="D28" s="27"/>
+      <c r="E28" s="28"/>
+      <c r="F28" s="32"/>
       <c r="G28" s="22"/>
       <c r="H28" s="22"/>
-      <c r="I28" s="31"/>
+      <c r="I28" s="30"/>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="28"/>
-      <c r="B29" s="28"/>
-      <c r="C29" s="28"/>
-      <c r="D29" s="28"/>
-      <c r="E29" s="29"/>
-      <c r="F29" s="33"/>
+      <c r="A29" s="25"/>
+      <c r="B29" s="26"/>
+      <c r="C29" s="26"/>
+      <c r="D29" s="27"/>
+      <c r="E29" s="28"/>
+      <c r="F29" s="32"/>
       <c r="G29" s="22"/>
       <c r="H29" s="22"/>
-      <c r="I29" s="31"/>
+      <c r="I29" s="30"/>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="26"/>
-      <c r="B30" s="27"/>
-      <c r="C30" s="27"/>
-      <c r="D30" s="28"/>
-      <c r="E30" s="29"/>
-      <c r="F30" s="33"/>
+      <c r="A30" s="25"/>
+      <c r="B30" s="26"/>
+      <c r="C30" s="26"/>
+      <c r="D30" s="27"/>
+      <c r="E30" s="31"/>
+      <c r="F30" s="32"/>
       <c r="G30" s="22"/>
       <c r="H30" s="22"/>
-      <c r="I30" s="31"/>
+      <c r="I30" s="30"/>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="26"/>
-      <c r="B31" s="27"/>
-      <c r="C31" s="27"/>
-      <c r="D31" s="28"/>
-      <c r="E31" s="32"/>
+      <c r="A31" s="25"/>
+      <c r="B31" s="26"/>
+      <c r="C31" s="26"/>
+      <c r="D31" s="27"/>
+      <c r="E31" s="31"/>
       <c r="F31" s="33"/>
       <c r="G31" s="22"/>
       <c r="H31" s="22"/>
-      <c r="I31" s="31"/>
+      <c r="I31" s="30"/>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="26"/>
+      <c r="A32" s="27"/>
       <c r="B32" s="27"/>
       <c r="C32" s="27"/>
-      <c r="D32" s="28"/>
-      <c r="E32" s="32"/>
-      <c r="F32" s="34"/>
+      <c r="D32" s="27"/>
+      <c r="E32" s="28"/>
+      <c r="F32" s="32"/>
       <c r="G32" s="22"/>
       <c r="H32" s="22"/>
-      <c r="I32" s="31"/>
+      <c r="I32" s="30"/>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="28"/>
-      <c r="B33" s="28"/>
-      <c r="C33" s="28"/>
-      <c r="D33" s="28"/>
-      <c r="E33" s="29"/>
-      <c r="F33" s="33"/>
+      <c r="A33" s="27"/>
+      <c r="B33" s="27"/>
+      <c r="C33" s="27"/>
+      <c r="D33" s="27"/>
+      <c r="E33" s="28"/>
+      <c r="F33" s="32"/>
       <c r="G33" s="22"/>
       <c r="H33" s="22"/>
-      <c r="I33" s="31"/>
+      <c r="I33" s="30"/>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="28"/>
-      <c r="B34" s="28"/>
-      <c r="C34" s="28"/>
-      <c r="D34" s="28"/>
-      <c r="E34" s="29"/>
-      <c r="F34" s="33"/>
+      <c r="A34" s="25"/>
+      <c r="B34" s="26"/>
+      <c r="C34" s="26"/>
+      <c r="D34" s="26"/>
+      <c r="E34" s="31"/>
+      <c r="F34" s="32"/>
       <c r="G34" s="22"/>
       <c r="H34" s="22"/>
-      <c r="I34" s="31"/>
+      <c r="I34" s="30"/>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="26"/>
+      <c r="A35" s="27"/>
       <c r="B35" s="27"/>
       <c r="C35" s="27"/>
       <c r="D35" s="27"/>
-      <c r="E35" s="32"/>
-      <c r="F35" s="33"/>
+      <c r="E35" s="28"/>
+      <c r="F35" s="32"/>
       <c r="G35" s="22"/>
       <c r="H35" s="22"/>
-      <c r="I35" s="31"/>
+      <c r="I35" s="30"/>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="28"/>
-      <c r="B36" s="28"/>
-      <c r="C36" s="28"/>
-      <c r="D36" s="28"/>
-      <c r="E36" s="29"/>
-      <c r="F36" s="33"/>
+      <c r="A36" s="27"/>
+      <c r="B36" s="27"/>
+      <c r="C36" s="27"/>
+      <c r="D36" s="27"/>
+      <c r="E36" s="28"/>
+      <c r="F36" s="32"/>
       <c r="G36" s="22"/>
       <c r="H36" s="22"/>
-      <c r="I36" s="31"/>
+      <c r="I36" s="30"/>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="28"/>
-      <c r="B37" s="28"/>
-      <c r="C37" s="28"/>
-      <c r="D37" s="28"/>
-      <c r="E37" s="29"/>
-      <c r="F37" s="33"/>
+      <c r="A37" s="27"/>
+      <c r="B37" s="27"/>
+      <c r="C37" s="27"/>
+      <c r="D37" s="27"/>
+      <c r="E37" s="28"/>
+      <c r="F37" s="32"/>
       <c r="G37" s="22"/>
       <c r="H37" s="22"/>
-      <c r="I37" s="31"/>
+      <c r="I37" s="30"/>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="28"/>
-      <c r="B38" s="28"/>
-      <c r="C38" s="28"/>
-      <c r="D38" s="28"/>
-      <c r="E38" s="29"/>
-      <c r="F38" s="33"/>
+      <c r="A38" s="27"/>
+      <c r="B38" s="27"/>
+      <c r="C38" s="27"/>
+      <c r="D38" s="27"/>
+      <c r="E38" s="28"/>
+      <c r="F38" s="32"/>
       <c r="G38" s="22"/>
       <c r="H38" s="22"/>
-      <c r="I38" s="31"/>
+      <c r="I38" s="30"/>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="28"/>
-      <c r="B39" s="28"/>
-      <c r="C39" s="28"/>
-      <c r="D39" s="28"/>
-      <c r="E39" s="29"/>
-      <c r="F39" s="33"/>
+      <c r="A39" s="27"/>
+      <c r="B39" s="27"/>
+      <c r="C39" s="27"/>
+      <c r="D39" s="27"/>
+      <c r="E39" s="28"/>
+      <c r="F39" s="32"/>
       <c r="G39" s="22"/>
       <c r="H39" s="22"/>
-      <c r="I39" s="31"/>
+      <c r="I39" s="30"/>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="28"/>
-      <c r="B40" s="28"/>
-      <c r="C40" s="28"/>
-      <c r="D40" s="28"/>
-      <c r="E40" s="29"/>
-      <c r="F40" s="33"/>
+      <c r="A40" s="27"/>
+      <c r="B40" s="27"/>
+      <c r="C40" s="27"/>
+      <c r="D40" s="27"/>
+      <c r="E40" s="28"/>
+      <c r="F40" s="32"/>
       <c r="G40" s="22"/>
       <c r="H40" s="22"/>
-      <c r="I40" s="31"/>
+      <c r="I40" s="30"/>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="28"/>
-      <c r="B41" s="28"/>
-      <c r="C41" s="28"/>
-      <c r="D41" s="28"/>
-      <c r="E41" s="29"/>
-      <c r="F41" s="33"/>
+      <c r="A41" s="27"/>
+      <c r="B41" s="27"/>
+      <c r="C41" s="27"/>
+      <c r="D41" s="27"/>
+      <c r="E41" s="28"/>
+      <c r="F41" s="32"/>
       <c r="G41" s="22"/>
       <c r="H41" s="22"/>
-      <c r="I41" s="31"/>
+      <c r="I41" s="30"/>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="28"/>
-      <c r="B42" s="28"/>
-      <c r="C42" s="28"/>
-      <c r="D42" s="28"/>
-      <c r="E42" s="29"/>
-      <c r="F42" s="33"/>
+      <c r="A42" s="27"/>
+      <c r="B42" s="27"/>
+      <c r="C42" s="27"/>
+      <c r="D42" s="27"/>
+      <c r="E42" s="28"/>
+      <c r="F42" s="32"/>
       <c r="G42" s="22"/>
       <c r="H42" s="22"/>
-      <c r="I42" s="31"/>
+      <c r="I42" s="30"/>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="28"/>
-      <c r="B43" s="28"/>
-      <c r="C43" s="28"/>
-      <c r="D43" s="28"/>
-      <c r="E43" s="29"/>
-      <c r="F43" s="33"/>
+      <c r="A43" s="27"/>
+      <c r="B43" s="27"/>
+      <c r="C43" s="27"/>
+      <c r="D43" s="27"/>
+      <c r="E43" s="28"/>
+      <c r="F43" s="32"/>
       <c r="G43" s="22"/>
       <c r="H43" s="22"/>
-      <c r="I43" s="31"/>
+      <c r="I43" s="30"/>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="28"/>
-      <c r="B44" s="28"/>
-      <c r="C44" s="28"/>
-      <c r="D44" s="28"/>
-      <c r="E44" s="29"/>
-      <c r="F44" s="33"/>
+      <c r="A44" s="27"/>
+      <c r="B44" s="27"/>
+      <c r="C44" s="27"/>
+      <c r="D44" s="27"/>
+      <c r="E44" s="28"/>
+      <c r="F44" s="32"/>
       <c r="G44" s="22"/>
       <c r="H44" s="22"/>
-      <c r="I44" s="31"/>
+      <c r="I44" s="30"/>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="28"/>
-      <c r="B45" s="28"/>
-      <c r="C45" s="28"/>
-      <c r="D45" s="28"/>
-      <c r="E45" s="29"/>
-      <c r="F45" s="33"/>
+      <c r="A45" s="27"/>
+      <c r="B45" s="27"/>
+      <c r="C45" s="27"/>
+      <c r="D45" s="27"/>
+      <c r="E45" s="28"/>
+      <c r="F45" s="32"/>
       <c r="G45" s="22"/>
       <c r="H45" s="22"/>
-      <c r="I45" s="31"/>
+      <c r="I45" s="30"/>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="28"/>
-      <c r="B46" s="28"/>
-      <c r="C46" s="28"/>
-      <c r="D46" s="28"/>
-      <c r="E46" s="29"/>
-      <c r="F46" s="33"/>
+      <c r="A46" s="27"/>
+      <c r="B46" s="27"/>
+      <c r="C46" s="27"/>
+      <c r="D46" s="27"/>
+      <c r="E46" s="28"/>
+      <c r="F46" s="32"/>
       <c r="G46" s="22"/>
       <c r="H46" s="22"/>
-      <c r="I46" s="31"/>
+      <c r="I46" s="30"/>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="28"/>
-      <c r="B47" s="28"/>
-      <c r="C47" s="28"/>
-      <c r="D47" s="28"/>
-      <c r="E47" s="29"/>
-      <c r="F47" s="33"/>
+      <c r="A47" s="27"/>
+      <c r="B47" s="27"/>
+      <c r="C47" s="27"/>
+      <c r="D47" s="27"/>
+      <c r="E47" s="28"/>
+      <c r="F47" s="32"/>
       <c r="G47" s="22"/>
       <c r="H47" s="22"/>
-      <c r="I47" s="31"/>
-    </row>
-    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="28"/>
-      <c r="B48" s="28"/>
-      <c r="C48" s="28"/>
-      <c r="D48" s="28"/>
-      <c r="E48" s="29"/>
-      <c r="F48" s="33"/>
-      <c r="G48" s="22"/>
-      <c r="H48" s="22"/>
-      <c r="I48" s="31"/>
-    </row>
+      <c r="I47" s="30"/>
+    </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <conditionalFormatting sqref="G1">
     <cfRule type="cellIs" priority="2" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
@@ -1748,12 +1695,12 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="G1:G1048" type="list">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="G1:G1047" type="list">
       <formula1>$K$4:$K$5</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="H1:H1048" type="list">
-      <formula1>$K$8:$K$9</formula1>
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="H1:H1047" type="list">
+      <formula1>$K$8:$K$8</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Add CYRS & HSI Review sheets Signed-off-by: Abdelrahman-Omar-Ali <a.abdelwahed20@gmail.com>
</commit_message>
<xml_diff>
--- a/Input documents/CYRS_Review.xlsx
+++ b/Input documents/CYRS_Review.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="50">
   <si>
     <t xml:space="preserve">Project Name </t>
   </si>
@@ -140,7 +140,7 @@
     <t xml:space="preserve">Update Table of Content numbering specially for Functional Requirements section. </t>
   </si>
   <si>
-    <t xml:space="preserve">ALL</t>
+    <t xml:space="preserve">All</t>
   </si>
   <si>
     <t xml:space="preserve">There is no Reference table for the reference document , even CYRS should have one and the reference is the customer Requirement for the product </t>
@@ -155,9 +155,6 @@
     <t xml:space="preserve">You need to make your requirement more clarified from the system level prospective. 
 In REQ_PO2EBL_CYRS_02_V02 instead of saying when the switch is pressed again, the blender shall operate on the higher speed level until it reaches the maximum level, and the next press shall turn it off.
 You can say: the blender shall operate between 3 different speeds (Speed1 → Speed 2 → Speed 3) triggered by a button press after the fourth press it returns back to its initial state (off).  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">ALL </t>
   </si>
   <si>
     <r>
@@ -556,12 +553,12 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="10" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="7" fillId="0" borderId="10" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="10" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -748,7 +745,7 @@
       <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="32.29"/>
   </cols>
@@ -990,10 +987,10 @@
   <dimension ref="A1:L1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
+      <selection pane="topLeft" activeCell="F17" activeCellId="0" sqref="F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.71"/>
@@ -1131,10 +1128,10 @@
       <c r="D5" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="E5" s="20" t="s">
+      <c r="E5" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="F5" s="23" t="s">
+      <c r="F5" s="24" t="s">
         <v>39</v>
       </c>
       <c r="G5" s="22" t="s">
@@ -1149,7 +1146,7 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="64.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="24" t="s">
+      <c r="A6" s="17" t="s">
         <v>26</v>
       </c>
       <c r="B6" s="18" t="s">
@@ -1164,7 +1161,7 @@
       <c r="E6" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="F6" s="23" t="s">
+      <c r="F6" s="24" t="s">
         <v>42</v>
       </c>
       <c r="G6" s="22" t="s">
@@ -1176,7 +1173,7 @@
       <c r="I6" s="22"/>
     </row>
     <row r="7" customFormat="false" ht="52.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="24" t="s">
+      <c r="A7" s="17" t="s">
         <v>26</v>
       </c>
       <c r="B7" s="18" t="s">
@@ -1189,10 +1186,10 @@
         <v>29</v>
       </c>
       <c r="E7" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="F7" s="24" t="s">
         <v>43</v>
-      </c>
-      <c r="F7" s="23" t="s">
-        <v>44</v>
       </c>
       <c r="G7" s="22" t="s">
         <v>32</v>
@@ -1202,8 +1199,8 @@
       </c>
       <c r="I7" s="20"/>
     </row>
-    <row r="8" customFormat="false" ht="57.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="24" t="s">
+    <row r="8" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="17" t="s">
         <v>26</v>
       </c>
       <c r="B8" s="18" t="s">
@@ -1219,7 +1216,7 @@
         <v>38</v>
       </c>
       <c r="F8" s="21" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G8" s="22" t="s">
         <v>32</v>
@@ -1229,7 +1226,7 @@
       </c>
       <c r="I8" s="20"/>
       <c r="K8" s="0" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1265,10 +1262,10 @@
       <c r="H11" s="22"/>
       <c r="I11" s="20"/>
       <c r="K11" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="L11" s="0" t="s">
         <v>47</v>
-      </c>
-      <c r="L11" s="0" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1282,10 +1279,10 @@
       <c r="H12" s="22"/>
       <c r="I12" s="20"/>
       <c r="K12" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="L12" s="0" t="s">
         <v>49</v>
-      </c>
-      <c r="L12" s="0" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Update project plan and CYRS
Signed-off-by: Mohammmedibra96 <mohammedibra96@gmail.com>
</commit_message>
<xml_diff>
--- a/Input documents/CYRS_Review.xlsx
+++ b/Input documents/CYRS_Review.xlsx
@@ -1,20 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ITI\software\project\Input documents\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Introduction " sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Cross review points " sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Introduction " sheetId="1" r:id="rId1"/>
+    <sheet name="Cross review points " sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="false" localSheetId="1" name="_Toc30697436" vbProcedure="false">#REF!</definedName>
+    <definedName name="_Toc30697436" localSheetId="1">#REF!</definedName>
   </definedNames>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -41,28 +45,28 @@
     <t xml:space="preserve">Ref Version </t>
   </si>
   <si>
-    <t xml:space="preserve">V1.2</t>
+    <t>V1.2</t>
   </si>
   <si>
     <t xml:space="preserve">Auther </t>
   </si>
   <si>
-    <t xml:space="preserve">Tarek Sharaby</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Last update</t>
-  </si>
-  <si>
-    <t xml:space="preserve">24/01/2020</t>
-  </si>
-  <si>
-    <t xml:space="preserve">History</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Version</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Auther</t>
+    <t>Tarek Sharaby</t>
+  </si>
+  <si>
+    <t>Last update</t>
+  </si>
+  <si>
+    <t>24/01/2020</t>
+  </si>
+  <si>
+    <t>History</t>
+  </si>
+  <si>
+    <t>Version</t>
+  </si>
+  <si>
+    <t>Auther</t>
   </si>
   <si>
     <t xml:space="preserve">Date </t>
@@ -71,85 +75,85 @@
     <t xml:space="preserve">Change </t>
   </si>
   <si>
-    <t xml:space="preserve">T.Sharaby</t>
+    <t>T.Sharaby</t>
   </si>
   <si>
     <t xml:space="preserve">Initial creation </t>
   </si>
   <si>
-    <t xml:space="preserve">Entry Date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reviewer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Detection version</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Name of file</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Page/Line/Section/Entity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Open point : description of problem</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Decision</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Status</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Comment</t>
-  </si>
-  <si>
-    <t xml:space="preserve">29/01/2020</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A.Ali</t>
-  </si>
-  <si>
-    <t xml:space="preserve">V0.2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CYRS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Page 1</t>
+    <t>Entry Date</t>
+  </si>
+  <si>
+    <t>Reviewer</t>
+  </si>
+  <si>
+    <t>Detection version</t>
+  </si>
+  <si>
+    <t>Name of file</t>
+  </si>
+  <si>
+    <t>Page/Line/Section/Entity</t>
+  </si>
+  <si>
+    <t>Open point : description of problem</t>
+  </si>
+  <si>
+    <t>Decision</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Comment</t>
+  </si>
+  <si>
+    <t>29/01/2020</t>
+  </si>
+  <si>
+    <t>A.Ali</t>
+  </si>
+  <si>
+    <t>V0.2</t>
+  </si>
+  <si>
+    <t>CYRS</t>
+  </si>
+  <si>
+    <t>Page 1</t>
   </si>
   <si>
     <t xml:space="preserve">Status of document must be changed from Draft to Proposed and then Releases after accomplishing cross review on it. </t>
   </si>
   <si>
-    <t xml:space="preserve">Accepted</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Open</t>
-  </si>
-  <si>
-    <t xml:space="preserve">All pages</t>
+    <t>Accepted</t>
+  </si>
+  <si>
+    <t>Open</t>
+  </si>
+  <si>
+    <t>All pages</t>
   </si>
   <si>
     <t xml:space="preserve">Redundancy in Version field besides Date in header table. </t>
   </si>
   <si>
-    <t xml:space="preserve">Contents</t>
+    <t>Contents</t>
   </si>
   <si>
     <t xml:space="preserve">Update Table of Content numbering specially for Functional Requirements section. </t>
   </si>
   <si>
-    <t xml:space="preserve">All</t>
+    <t>All</t>
   </si>
   <si>
     <t xml:space="preserve">There is no Reference table for the reference document , even CYRS should have one and the reference is the customer Requirement for the product </t>
   </si>
   <si>
-    <t xml:space="preserve">Refused</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Functional Requirements</t>
+    <t>Refused</t>
+  </si>
+  <si>
+    <t>Functional Requirements</t>
   </si>
   <si>
     <t xml:space="preserve">You need to make your requirement more clarified from the system level prospective. 
@@ -165,7 +169,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">REQ_PO2EBL_CYRS_03_V02 :</t>
+      <t>REQ_PO2EBL_CYRS_03_V02 :</t>
     </r>
     <r>
       <rPr>
@@ -193,7 +197,7 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">Resolved</t>
+    <t>Resolved</t>
   </si>
   <si>
     <t xml:space="preserve">Decision </t>
@@ -211,15 +215,13 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="5">
-    <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="DD/MM/YY;@"/>
-    <numFmt numFmtId="166" formatCode="[$-409]General"/>
-    <numFmt numFmtId="167" formatCode="[$-409]M/D/YYYY"/>
-    <numFmt numFmtId="168" formatCode="@"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="3">
+    <numFmt numFmtId="164" formatCode="dd/mm/yy;@"/>
+    <numFmt numFmtId="165" formatCode="[$-409]General"/>
+    <numFmt numFmtId="166" formatCode="[$-409]m/d/yyyy"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -228,22 +230,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <b val="true"/>
+      <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -251,7 +238,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
@@ -279,6 +266,13 @@
     </font>
     <font>
       <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -312,103 +306,149 @@
     </fill>
   </fills>
   <borders count="11">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left style="medium">
         <color rgb="FF70AD47"/>
       </left>
-      <right style="thin"/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
       <top style="medium">
         <color rgb="FF70AD47"/>
       </top>
-      <bottom style="thin"/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
       <right style="medium">
         <color rgb="FF70AD47"/>
       </right>
       <top style="medium">
         <color rgb="FF70AD47"/>
       </top>
-      <bottom style="thin"/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
       <right style="medium">
         <color rgb="FF70AD47"/>
       </right>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left style="medium">
         <color rgb="FF70AD47"/>
       </left>
       <right style="medium">
         <color rgb="FF70AD47"/>
       </right>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left style="medium">
         <color rgb="FF70AD47"/>
       </left>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left style="medium">
         <color rgb="FF70AD47"/>
       </left>
-      <right style="thin"/>
-      <top style="thin"/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
       <bottom style="medium">
         <color rgb="FF70AD47"/>
       </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
       <bottom style="medium">
         <color rgb="FF70AD47"/>
       </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
       <right style="medium">
         <color rgb="FF70AD47"/>
       </right>
-      <top style="thin"/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
       <bottom style="medium">
         <color rgb="FF70AD47"/>
       </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -424,207 +464,154 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="23">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
+  <cellStyleXfs count="4">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="34">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="3" borderId="10" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="10" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="3" borderId="10" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="10" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="10" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="10" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="10" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="10" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="10" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="10" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="10" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="10" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="10" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="10" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="10" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="10" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="10" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="10" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="9">
+  <cellStyles count="4">
+    <cellStyle name="Excel Built-in Accent3" xfId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
-    <cellStyle name="Normal 3 2" xfId="20"/>
-    <cellStyle name="Normal 4" xfId="21"/>
-    <cellStyle name="Excel Built-in Accent3" xfId="22"/>
+    <cellStyle name="Normal 3 2" xfId="1"/>
+    <cellStyle name="Normal 4" xfId="2"/>
   </cellStyles>
   <dxfs count="5">
     <dxf>
       <font>
-        <b val="1"/>
+        <b/>
         <i val="0"/>
-        <color rgb="FF808080"/>
+        <color rgb="FFFBE5D6"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFF2F2F2"/>
+          <bgColor rgb="FFC00000"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <font>
-        <b val="1"/>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF1F4E79"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDAE3F3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF385724"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
         <i val="0"/>
         <color rgb="FF535353"/>
       </font>
@@ -636,41 +623,18 @@
     </dxf>
     <dxf>
       <font>
-        <b val="1"/>
+        <b/>
         <i val="0"/>
-        <color rgb="FF385724"/>
+        <color rgb="FF808080"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFFFCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="1"/>
-        <i val="0"/>
-        <color rgb="FF1F4E79"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDAE3F3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="1"/>
-        <i val="0"/>
-        <color rgb="FFFBE5D6"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC00000"/>
+          <bgColor rgb="FFF2F2F2"/>
         </patternFill>
       </fill>
     </dxf>
   </dxfs>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -729,223 +693,500 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF1F4E79"/>
       <rgbColor rgb="FF385724"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4472C4"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="B2:H18"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B3:H18"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="32.29"/>
+    <col min="8" max="8" width="32.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="1" t="s">
+    <row r="3" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B3" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="2" t="s">
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-    </row>
-    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-    </row>
-    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="1" t="s">
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B4" s="10"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="9"/>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B5" s="10"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9"/>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B6" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="1"/>
-      <c r="D6" s="3" t="s">
+      <c r="C6" s="10"/>
+      <c r="D6" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-    </row>
-    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="1" t="s">
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8"/>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B7" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="1"/>
-      <c r="D7" s="3" t="s">
+      <c r="C7" s="10"/>
+      <c r="D7" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-    </row>
-    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="1" t="s">
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B8" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="1"/>
-      <c r="D8" s="3" t="s">
+      <c r="C8" s="10"/>
+      <c r="D8" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="1" t="s">
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="8"/>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B9" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="1"/>
-      <c r="D9" s="3" t="s">
+      <c r="C9" s="10"/>
+      <c r="D9" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="5" t="s">
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B11" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
-      <c r="H11" s="5"/>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="6" t="s">
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B12" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="C12" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D12" s="7"/>
-      <c r="E12" s="7" t="s">
+      <c r="D12" s="5"/>
+      <c r="E12" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="F12" s="7"/>
-      <c r="G12" s="8" t="s">
+      <c r="F12" s="5"/>
+      <c r="G12" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="H12" s="8"/>
-    </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="9" t="n">
+      <c r="H12" s="4"/>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B13" s="12">
         <v>0.1</v>
       </c>
-      <c r="C13" s="10" t="s">
+      <c r="C13" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D13" s="10"/>
-      <c r="E13" s="10" t="s">
+      <c r="D13" s="3"/>
+      <c r="E13" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F13" s="10"/>
-      <c r="G13" s="3" t="s">
+      <c r="F13" s="3"/>
+      <c r="G13" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="H13" s="3"/>
-    </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="9"/>
-      <c r="C14" s="10"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="10"/>
-      <c r="F14" s="10"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
-    </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="9"/>
-      <c r="C15" s="10"/>
-      <c r="D15" s="10"/>
-      <c r="E15" s="10"/>
-      <c r="F15" s="10"/>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
-    </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="9"/>
-      <c r="C16" s="10"/>
-      <c r="D16" s="10"/>
-      <c r="E16" s="10"/>
-      <c r="F16" s="10"/>
-      <c r="G16" s="3"/>
-      <c r="H16" s="3"/>
-    </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="9"/>
-      <c r="C17" s="10"/>
-      <c r="D17" s="10"/>
-      <c r="E17" s="10"/>
-      <c r="F17" s="10"/>
-      <c r="G17" s="3"/>
-      <c r="H17" s="3"/>
-    </row>
-    <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="11"/>
-      <c r="C18" s="12"/>
-      <c r="D18" s="12"/>
-      <c r="E18" s="12"/>
-      <c r="F18" s="12"/>
-      <c r="G18" s="13"/>
-      <c r="H18" s="13"/>
+      <c r="H13" s="8"/>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B14" s="12"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="8"/>
+      <c r="H14" s="8"/>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B15" s="12"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="8"/>
+      <c r="H15" s="8"/>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B16" s="12"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="8"/>
+      <c r="H16" s="8"/>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B17" s="12"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="8"/>
+      <c r="H17" s="8"/>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B18" s="13"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="33">
-    <mergeCell ref="B3:D5"/>
-    <mergeCell ref="E3:H5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="D6:H6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="D7:H7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="D8:H8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="D9:H9"/>
-    <mergeCell ref="B10:H10"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="G15:H15"/>
     <mergeCell ref="B11:H11"/>
     <mergeCell ref="C12:D12"/>
     <mergeCell ref="E12:F12"/>
@@ -953,56 +1194,44 @@
     <mergeCell ref="C13:D13"/>
     <mergeCell ref="E13:F13"/>
     <mergeCell ref="G13:H13"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="G16:H16"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="G17:H17"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="D8:H8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="D9:H9"/>
+    <mergeCell ref="B10:H10"/>
+    <mergeCell ref="B3:D5"/>
+    <mergeCell ref="E3:H5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="D6:H6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D7:H7"/>
   </mergeCells>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:L1048576"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L47"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F17" activeCellId="0" sqref="F17"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="11.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="24"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="100.41"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="8" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="174.28"/>
+    <col min="1" max="1" width="10.54296875" customWidth="1"/>
+    <col min="2" max="2" width="8.7265625" customWidth="1"/>
+    <col min="3" max="3" width="15.26953125" customWidth="1"/>
+    <col min="4" max="4" width="11.54296875" customWidth="1"/>
+    <col min="5" max="5" width="24" customWidth="1"/>
+    <col min="6" max="6" width="100.36328125" customWidth="1"/>
+    <col min="8" max="9" width="11.54296875" customWidth="1"/>
+    <col min="12" max="12" width="174.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="34.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:12" ht="34.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="14" t="s">
         <v>17</v>
       </c>
@@ -1031,7 +1260,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" s="17" t="s">
         <v>26</v>
       </c>
@@ -1058,7 +1287,7 @@
       </c>
       <c r="I2" s="22"/>
     </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" s="17" t="s">
         <v>26</v>
       </c>
@@ -1085,7 +1314,7 @@
       </c>
       <c r="I3" s="22"/>
     </row>
-    <row r="4" customFormat="false" ht="20.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:12" ht="20.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="17" t="s">
         <v>26</v>
       </c>
@@ -1111,11 +1340,11 @@
         <v>33</v>
       </c>
       <c r="I4" s="22"/>
-      <c r="K4" s="0" t="s">
+      <c r="K4" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="A5" s="17" t="s">
         <v>26</v>
       </c>
@@ -1141,11 +1370,11 @@
         <v>33</v>
       </c>
       <c r="I5" s="22"/>
-      <c r="K5" s="0" t="s">
+      <c r="K5" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="64.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:12" ht="64.900000000000006" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="17" t="s">
         <v>26</v>
       </c>
@@ -1172,7 +1401,7 @@
       </c>
       <c r="I6" s="22"/>
     </row>
-    <row r="7" customFormat="false" ht="52.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:12" ht="52.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="17" t="s">
         <v>26</v>
       </c>
@@ -1199,7 +1428,7 @@
       </c>
       <c r="I7" s="20"/>
     </row>
-    <row r="8" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:12" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A8" s="17" t="s">
         <v>26</v>
       </c>
@@ -1225,11 +1454,11 @@
         <v>33</v>
       </c>
       <c r="I8" s="20"/>
-      <c r="K8" s="0" t="s">
+      <c r="K8" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A9" s="17"/>
       <c r="B9" s="18"/>
       <c r="C9" s="19"/>
@@ -1240,7 +1469,7 @@
       <c r="H9" s="22"/>
       <c r="I9" s="20"/>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A10" s="18"/>
       <c r="B10" s="18"/>
       <c r="C10" s="19"/>
@@ -1251,7 +1480,7 @@
       <c r="H10" s="22"/>
       <c r="I10" s="20"/>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A11" s="18"/>
       <c r="B11" s="18"/>
       <c r="C11" s="19"/>
@@ -1261,14 +1490,14 @@
       <c r="G11" s="22"/>
       <c r="H11" s="22"/>
       <c r="I11" s="20"/>
-      <c r="K11" s="0" t="s">
+      <c r="K11" t="s">
         <v>46</v>
       </c>
-      <c r="L11" s="0" t="s">
+      <c r="L11" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A12" s="18"/>
       <c r="B12" s="18"/>
       <c r="C12" s="19"/>
@@ -1278,14 +1507,14 @@
       <c r="G12" s="22"/>
       <c r="H12" s="22"/>
       <c r="I12" s="20"/>
-      <c r="K12" s="0" t="s">
+      <c r="K12" t="s">
         <v>48</v>
       </c>
-      <c r="L12" s="0" t="s">
+      <c r="L12" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A13" s="18"/>
       <c r="B13" s="18"/>
       <c r="C13" s="19"/>
@@ -1296,7 +1525,7 @@
       <c r="H13" s="22"/>
       <c r="I13" s="20"/>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A14" s="18"/>
       <c r="B14" s="18"/>
       <c r="C14" s="19"/>
@@ -1307,7 +1536,7 @@
       <c r="H14" s="22"/>
       <c r="I14" s="20"/>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A15" s="18"/>
       <c r="B15" s="18"/>
       <c r="C15" s="19"/>
@@ -1318,7 +1547,7 @@
       <c r="H15" s="22"/>
       <c r="I15" s="20"/>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A16" s="25"/>
       <c r="B16" s="26"/>
       <c r="C16" s="26"/>
@@ -1329,7 +1558,7 @@
       <c r="H16" s="22"/>
       <c r="I16" s="30"/>
     </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" s="25"/>
       <c r="B17" s="26"/>
       <c r="C17" s="26"/>
@@ -1340,7 +1569,7 @@
       <c r="H17" s="22"/>
       <c r="I17" s="30"/>
     </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" s="25"/>
       <c r="B18" s="26"/>
       <c r="C18" s="27"/>
@@ -1351,7 +1580,7 @@
       <c r="H18" s="22"/>
       <c r="I18" s="30"/>
     </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" s="25"/>
       <c r="B19" s="26"/>
       <c r="C19" s="27"/>
@@ -1362,7 +1591,7 @@
       <c r="H19" s="22"/>
       <c r="I19" s="30"/>
     </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20" s="25"/>
       <c r="B20" s="26"/>
       <c r="C20" s="27"/>
@@ -1373,7 +1602,7 @@
       <c r="H20" s="22"/>
       <c r="I20" s="30"/>
     </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21" s="25"/>
       <c r="B21" s="26"/>
       <c r="C21" s="27"/>
@@ -1384,7 +1613,7 @@
       <c r="H21" s="22"/>
       <c r="I21" s="30"/>
     </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22" s="25"/>
       <c r="B22" s="26"/>
       <c r="C22" s="27"/>
@@ -1395,7 +1624,7 @@
       <c r="H22" s="22"/>
       <c r="I22" s="30"/>
     </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23" s="25"/>
       <c r="B23" s="26"/>
       <c r="C23" s="27"/>
@@ -1406,7 +1635,7 @@
       <c r="H23" s="22"/>
       <c r="I23" s="30"/>
     </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24" s="25"/>
       <c r="B24" s="26"/>
       <c r="C24" s="27"/>
@@ -1417,7 +1646,7 @@
       <c r="H24" s="22"/>
       <c r="I24" s="30"/>
     </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25" s="25"/>
       <c r="B25" s="26"/>
       <c r="C25" s="27"/>
@@ -1428,7 +1657,7 @@
       <c r="H25" s="22"/>
       <c r="I25" s="30"/>
     </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A26" s="25"/>
       <c r="B26" s="26"/>
       <c r="C26" s="27"/>
@@ -1439,7 +1668,7 @@
       <c r="H26" s="22"/>
       <c r="I26" s="30"/>
     </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A27" s="25"/>
       <c r="B27" s="26"/>
       <c r="C27" s="27"/>
@@ -1450,7 +1679,7 @@
       <c r="H27" s="22"/>
       <c r="I27" s="30"/>
     </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A28" s="27"/>
       <c r="B28" s="27"/>
       <c r="C28" s="27"/>
@@ -1461,7 +1690,7 @@
       <c r="H28" s="22"/>
       <c r="I28" s="30"/>
     </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A29" s="25"/>
       <c r="B29" s="26"/>
       <c r="C29" s="26"/>
@@ -1472,7 +1701,7 @@
       <c r="H29" s="22"/>
       <c r="I29" s="30"/>
     </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A30" s="25"/>
       <c r="B30" s="26"/>
       <c r="C30" s="26"/>
@@ -1483,7 +1712,7 @@
       <c r="H30" s="22"/>
       <c r="I30" s="30"/>
     </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A31" s="25"/>
       <c r="B31" s="26"/>
       <c r="C31" s="26"/>
@@ -1494,7 +1723,7 @@
       <c r="H31" s="22"/>
       <c r="I31" s="30"/>
     </row>
-    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A32" s="27"/>
       <c r="B32" s="27"/>
       <c r="C32" s="27"/>
@@ -1505,7 +1734,7 @@
       <c r="H32" s="22"/>
       <c r="I32" s="30"/>
     </row>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A33" s="27"/>
       <c r="B33" s="27"/>
       <c r="C33" s="27"/>
@@ -1516,7 +1745,7 @@
       <c r="H33" s="22"/>
       <c r="I33" s="30"/>
     </row>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A34" s="25"/>
       <c r="B34" s="26"/>
       <c r="C34" s="26"/>
@@ -1527,7 +1756,7 @@
       <c r="H34" s="22"/>
       <c r="I34" s="30"/>
     </row>
-    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A35" s="27"/>
       <c r="B35" s="27"/>
       <c r="C35" s="27"/>
@@ -1538,7 +1767,7 @@
       <c r="H35" s="22"/>
       <c r="I35" s="30"/>
     </row>
-    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A36" s="27"/>
       <c r="B36" s="27"/>
       <c r="C36" s="27"/>
@@ -1549,7 +1778,7 @@
       <c r="H36" s="22"/>
       <c r="I36" s="30"/>
     </row>
-    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A37" s="27"/>
       <c r="B37" s="27"/>
       <c r="C37" s="27"/>
@@ -1560,7 +1789,7 @@
       <c r="H37" s="22"/>
       <c r="I37" s="30"/>
     </row>
-    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A38" s="27"/>
       <c r="B38" s="27"/>
       <c r="C38" s="27"/>
@@ -1571,7 +1800,7 @@
       <c r="H38" s="22"/>
       <c r="I38" s="30"/>
     </row>
-    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A39" s="27"/>
       <c r="B39" s="27"/>
       <c r="C39" s="27"/>
@@ -1582,7 +1811,7 @@
       <c r="H39" s="22"/>
       <c r="I39" s="30"/>
     </row>
-    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A40" s="27"/>
       <c r="B40" s="27"/>
       <c r="C40" s="27"/>
@@ -1593,7 +1822,7 @@
       <c r="H40" s="22"/>
       <c r="I40" s="30"/>
     </row>
-    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A41" s="27"/>
       <c r="B41" s="27"/>
       <c r="C41" s="27"/>
@@ -1604,7 +1833,7 @@
       <c r="H41" s="22"/>
       <c r="I41" s="30"/>
     </row>
-    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A42" s="27"/>
       <c r="B42" s="27"/>
       <c r="C42" s="27"/>
@@ -1615,7 +1844,7 @@
       <c r="H42" s="22"/>
       <c r="I42" s="30"/>
     </row>
-    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A43" s="27"/>
       <c r="B43" s="27"/>
       <c r="C43" s="27"/>
@@ -1626,7 +1855,7 @@
       <c r="H43" s="22"/>
       <c r="I43" s="30"/>
     </row>
-    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A44" s="27"/>
       <c r="B44" s="27"/>
       <c r="C44" s="27"/>
@@ -1637,7 +1866,7 @@
       <c r="H44" s="22"/>
       <c r="I44" s="30"/>
     </row>
-    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A45" s="27"/>
       <c r="B45" s="27"/>
       <c r="C45" s="27"/>
@@ -1648,7 +1877,7 @@
       <c r="H45" s="22"/>
       <c r="I45" s="30"/>
     </row>
-    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A46" s="27"/>
       <c r="B46" s="27"/>
       <c r="C46" s="27"/>
@@ -1659,7 +1888,7 @@
       <c r="H46" s="22"/>
       <c r="I46" s="30"/>
     </row>
-    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A47" s="27"/>
       <c r="B47" s="27"/>
       <c r="C47" s="27"/>
@@ -1670,43 +1899,37 @@
       <c r="H47" s="22"/>
       <c r="I47" s="30"/>
     </row>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <conditionalFormatting sqref="G1">
-    <cfRule type="cellIs" priority="2" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
       <formula>$G$4</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="3" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
       <formula>$G$3</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="4" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
-      <formula>#ref!</formula>
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
+      <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="5" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
+    <cfRule type="cellIs" dxfId="1" priority="5" operator="equal">
       <formula>$G$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1">
-    <cfRule type="cellIs" priority="6" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
+    <cfRule type="cellIs" dxfId="0" priority="6" operator="equal">
       <formula>$G$4</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="G1:G1047" type="list">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G1:G1047">
       <formula1>$K$4:$K$5</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="H1:H1047" type="list">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H1:H1047">
       <formula1>$K$8:$K$8</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>